<commit_message>
update ISS Dec 4th
</commit_message>
<xml_diff>
--- a/data/computed/Rt_from_ISS_processed.xlsx
+++ b/data/computed/Rt_from_ISS_processed.xlsx
@@ -430,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -472,321 +472,341 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>44139</v>
+        <v>44146</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>44152</v>
+        <v>44159</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>44145.99998842592</v>
+        <v>44152.99998842592</v>
       </c>
       <c r="D2" t="n">
+        <v>0.91</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.79</v>
+      </c>
+      <c r="F2" t="n">
         <v>1.08</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0.91</v>
-      </c>
-      <c r="F2" t="n">
-        <v>1.25</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>44132</v>
+        <v>44139</v>
       </c>
       <c r="B3" s="2" t="n">
-        <v>44145</v>
+        <v>44152</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>44138.99998842592</v>
+        <v>44145.99998842592</v>
       </c>
       <c r="D3" t="n">
-        <v>1.18</v>
+        <v>1.08</v>
       </c>
       <c r="E3" t="n">
-        <v>0.9399999999999999</v>
+        <v>0.91</v>
       </c>
       <c r="F3" t="n">
-        <v>1.49</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>44126</v>
+        <v>44132</v>
       </c>
       <c r="B4" s="2" t="n">
-        <v>44139</v>
+        <v>44145</v>
       </c>
       <c r="C4" s="2" t="n">
-        <v>44132.99998842592</v>
+        <v>44138.99998842592</v>
       </c>
       <c r="D4" t="n">
-        <v>1.43</v>
+        <v>1.18</v>
       </c>
       <c r="E4" t="n">
-        <v>1.08</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="F4" t="n">
-        <v>1.81</v>
+        <v>1.49</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>44119</v>
+        <v>44126</v>
       </c>
       <c r="B5" s="2" t="n">
-        <v>44132</v>
+        <v>44139</v>
       </c>
       <c r="C5" s="2" t="n">
-        <v>44125.99998842592</v>
+        <v>44132.99998842592</v>
       </c>
       <c r="D5" t="n">
-        <v>1.72</v>
+        <v>1.43</v>
       </c>
       <c r="E5" t="n">
-        <v>1.45</v>
+        <v>1.08</v>
       </c>
       <c r="F5" t="n">
-        <v>1.83</v>
+        <v>1.81</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
-        <v>44112</v>
+        <v>44119</v>
       </c>
       <c r="B6" s="2" t="n">
-        <v>44125</v>
+        <v>44132</v>
       </c>
       <c r="C6" s="2" t="n">
-        <v>44118.99998842592</v>
+        <v>44125.99998842592</v>
       </c>
       <c r="D6" t="n">
-        <v>1.7</v>
+        <v>1.72</v>
       </c>
       <c r="E6" t="n">
-        <v>1.49</v>
+        <v>1.45</v>
       </c>
       <c r="F6" t="n">
-        <v>1.85</v>
+        <v>1.83</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
-        <v>44105</v>
+        <v>44112</v>
       </c>
       <c r="B7" s="2" t="n">
-        <v>44118</v>
+        <v>44125</v>
       </c>
       <c r="C7" s="2" t="n">
-        <v>44111.99998842592</v>
+        <v>44118.99998842592</v>
       </c>
       <c r="D7" t="n">
-        <v>1.5</v>
+        <v>1.7</v>
       </c>
       <c r="E7" t="n">
-        <v>1.09</v>
+        <v>1.49</v>
       </c>
       <c r="F7" t="n">
-        <v>1.75</v>
+        <v>1.85</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
-        <v>44098</v>
+        <v>44105</v>
       </c>
       <c r="B8" s="2" t="n">
-        <v>44111</v>
+        <v>44118</v>
       </c>
       <c r="C8" s="2" t="n">
-        <v>44104.99998842592</v>
+        <v>44111.99998842592</v>
       </c>
       <c r="D8" t="n">
-        <v>1.17</v>
+        <v>1.5</v>
       </c>
       <c r="E8" t="n">
-        <v>1.03</v>
+        <v>1.09</v>
       </c>
       <c r="F8" t="n">
-        <v>1.5</v>
+        <v>1.75</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
-        <v>44091</v>
+        <v>44098</v>
       </c>
       <c r="B9" s="2" t="n">
-        <v>44104</v>
+        <v>44111</v>
       </c>
       <c r="C9" s="2" t="n">
-        <v>44097.99998842592</v>
+        <v>44104.99998842592</v>
       </c>
       <c r="D9" t="n">
-        <v>1.06</v>
+        <v>1.17</v>
       </c>
       <c r="E9" t="n">
-        <v>0.97</v>
+        <v>1.03</v>
       </c>
       <c r="F9" t="n">
-        <v>1.16</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
-        <v>44084</v>
+        <v>44091</v>
       </c>
       <c r="B10" s="2" t="n">
-        <v>44097</v>
+        <v>44104</v>
       </c>
       <c r="C10" s="2" t="n">
-        <v>44090.99998842592</v>
+        <v>44097.99998842592</v>
       </c>
       <c r="D10" t="n">
-        <v>1.01</v>
+        <v>1.06</v>
       </c>
       <c r="E10" t="n">
-        <v>0.88</v>
+        <v>0.97</v>
       </c>
       <c r="F10" t="n">
-        <v>1.08</v>
+        <v>1.16</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
-        <v>44077</v>
+        <v>44084</v>
       </c>
       <c r="B11" s="2" t="n">
-        <v>44090</v>
+        <v>44097</v>
       </c>
       <c r="C11" s="2" t="n">
-        <v>44083.99998842592</v>
+        <v>44090.99998842592</v>
       </c>
       <c r="D11" t="n">
-        <v>0.95</v>
+        <v>1.01</v>
       </c>
       <c r="E11" t="n">
         <v>0.88</v>
       </c>
       <c r="F11" t="n">
-        <v>1.05</v>
+        <v>1.08</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
-        <v>44070</v>
+        <v>44077</v>
       </c>
       <c r="B12" s="2" t="n">
-        <v>44083</v>
+        <v>44090</v>
       </c>
       <c r="C12" s="2" t="n">
-        <v>44076.99998842592</v>
+        <v>44083.99998842592</v>
       </c>
       <c r="D12" t="n">
-        <v>0.92</v>
+        <v>0.95</v>
       </c>
       <c r="E12" t="n">
-        <v>0.79</v>
+        <v>0.88</v>
       </c>
       <c r="F12" t="n">
-        <v>1.17</v>
+        <v>1.05</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
-        <v>44063</v>
+        <v>44070</v>
       </c>
       <c r="B13" s="2" t="n">
-        <v>44076</v>
+        <v>44083</v>
       </c>
       <c r="C13" s="2" t="n">
-        <v>44069.99998842592</v>
+        <v>44076.99998842592</v>
       </c>
       <c r="D13" t="n">
-        <v>1.14</v>
+        <v>0.92</v>
       </c>
       <c r="E13" t="n">
-        <v>0.71</v>
+        <v>0.79</v>
       </c>
       <c r="F13" t="n">
-        <v>1.53</v>
+        <v>1.17</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
-        <v>44056</v>
+        <v>44063</v>
       </c>
       <c r="B14" s="2" t="n">
-        <v>44069</v>
+        <v>44076</v>
       </c>
       <c r="C14" s="2" t="n">
-        <v>44062.99998842592</v>
+        <v>44069.99998842592</v>
       </c>
       <c r="D14" t="n">
-        <v>1.18</v>
+        <v>1.14</v>
       </c>
       <c r="E14" t="n">
-        <v>0.86</v>
+        <v>0.71</v>
       </c>
       <c r="F14" t="n">
-        <v>1.43</v>
+        <v>1.53</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
-        <v>44049</v>
+        <v>44056</v>
       </c>
       <c r="B15" s="2" t="n">
-        <v>44062</v>
+        <v>44069</v>
       </c>
       <c r="C15" s="2" t="n">
-        <v>44055.99998842592</v>
+        <v>44062.99998842592</v>
       </c>
       <c r="D15" t="n">
-        <v>0.75</v>
+        <v>1.18</v>
       </c>
       <c r="E15" t="n">
-        <v>0.52</v>
+        <v>0.86</v>
       </c>
       <c r="F15" t="n">
-        <v>1.24</v>
+        <v>1.43</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
-        <v>44042</v>
+        <v>44049</v>
       </c>
       <c r="B16" s="2" t="n">
-        <v>44055</v>
+        <v>44062</v>
       </c>
       <c r="C16" s="2" t="n">
-        <v>44048.99998842592</v>
+        <v>44055.99998842592</v>
       </c>
       <c r="D16" t="n">
-        <v>0.83</v>
+        <v>0.75</v>
       </c>
       <c r="E16" t="n">
-        <v>0.67</v>
+        <v>0.52</v>
       </c>
       <c r="F16" t="n">
-        <v>1.06</v>
+        <v>1.24</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
+        <v>44042</v>
+      </c>
+      <c r="B17" s="2" t="n">
+        <v>44055</v>
+      </c>
+      <c r="C17" s="2" t="n">
+        <v>44048.99998842592</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0.83</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0.67</v>
+      </c>
+      <c r="F17" t="n">
+        <v>1.06</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="2" t="n">
         <v>44035</v>
       </c>
-      <c r="B17" s="2" t="n">
+      <c r="B18" s="2" t="n">
         <v>44048</v>
       </c>
-      <c r="C17" s="2" t="n">
+      <c r="C18" s="2" t="n">
         <v>44041.99998842592</v>
       </c>
-      <c r="D17" t="n">
+      <c r="D18" t="n">
         <v>0.96</v>
       </c>
-      <c r="E17" t="n">
+      <c r="E18" t="n">
         <v>0.75</v>
       </c>
-      <c r="F17" t="n">
+      <c r="F18" t="n">
         <v>1.2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ISS update Dec 12 2020
</commit_message>
<xml_diff>
--- a/data/computed/Rt_from_ISS_processed.xlsx
+++ b/data/computed/Rt_from_ISS_processed.xlsx
@@ -430,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -472,341 +472,361 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>44146</v>
+        <v>44153</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>44159</v>
+        <v>44166</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>44152.99998842592</v>
+        <v>44159.99998842592</v>
       </c>
       <c r="D2" t="n">
+        <v>0.82</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.76</v>
+      </c>
+      <c r="F2" t="n">
         <v>0.91</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0.79</v>
-      </c>
-      <c r="F2" t="n">
-        <v>1.08</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>44139</v>
+        <v>44146</v>
       </c>
       <c r="B3" s="2" t="n">
-        <v>44152</v>
+        <v>44159</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>44145.99998842592</v>
+        <v>44152.99998842592</v>
       </c>
       <c r="D3" t="n">
+        <v>0.91</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.79</v>
+      </c>
+      <c r="F3" t="n">
         <v>1.08</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0.91</v>
-      </c>
-      <c r="F3" t="n">
-        <v>1.25</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>44132</v>
+        <v>44139</v>
       </c>
       <c r="B4" s="2" t="n">
-        <v>44145</v>
+        <v>44152</v>
       </c>
       <c r="C4" s="2" t="n">
-        <v>44138.99998842592</v>
+        <v>44145.99998842592</v>
       </c>
       <c r="D4" t="n">
-        <v>1.18</v>
+        <v>1.08</v>
       </c>
       <c r="E4" t="n">
-        <v>0.9399999999999999</v>
+        <v>0.91</v>
       </c>
       <c r="F4" t="n">
-        <v>1.49</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>44126</v>
+        <v>44132</v>
       </c>
       <c r="B5" s="2" t="n">
-        <v>44139</v>
+        <v>44145</v>
       </c>
       <c r="C5" s="2" t="n">
-        <v>44132.99998842592</v>
+        <v>44138.99998842592</v>
       </c>
       <c r="D5" t="n">
-        <v>1.43</v>
+        <v>1.18</v>
       </c>
       <c r="E5" t="n">
-        <v>1.08</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="F5" t="n">
-        <v>1.81</v>
+        <v>1.49</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
-        <v>44119</v>
+        <v>44126</v>
       </c>
       <c r="B6" s="2" t="n">
-        <v>44132</v>
+        <v>44139</v>
       </c>
       <c r="C6" s="2" t="n">
-        <v>44125.99998842592</v>
+        <v>44132.99998842592</v>
       </c>
       <c r="D6" t="n">
-        <v>1.72</v>
+        <v>1.43</v>
       </c>
       <c r="E6" t="n">
-        <v>1.45</v>
+        <v>1.08</v>
       </c>
       <c r="F6" t="n">
-        <v>1.83</v>
+        <v>1.81</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
-        <v>44112</v>
+        <v>44119</v>
       </c>
       <c r="B7" s="2" t="n">
-        <v>44125</v>
+        <v>44132</v>
       </c>
       <c r="C7" s="2" t="n">
-        <v>44118.99998842592</v>
+        <v>44125.99998842592</v>
       </c>
       <c r="D7" t="n">
-        <v>1.7</v>
+        <v>1.72</v>
       </c>
       <c r="E7" t="n">
-        <v>1.49</v>
+        <v>1.45</v>
       </c>
       <c r="F7" t="n">
-        <v>1.85</v>
+        <v>1.83</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
-        <v>44105</v>
+        <v>44112</v>
       </c>
       <c r="B8" s="2" t="n">
-        <v>44118</v>
+        <v>44125</v>
       </c>
       <c r="C8" s="2" t="n">
-        <v>44111.99998842592</v>
+        <v>44118.99998842592</v>
       </c>
       <c r="D8" t="n">
-        <v>1.5</v>
+        <v>1.7</v>
       </c>
       <c r="E8" t="n">
-        <v>1.09</v>
+        <v>1.49</v>
       </c>
       <c r="F8" t="n">
-        <v>1.75</v>
+        <v>1.85</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
-        <v>44098</v>
+        <v>44105</v>
       </c>
       <c r="B9" s="2" t="n">
-        <v>44111</v>
+        <v>44118</v>
       </c>
       <c r="C9" s="2" t="n">
-        <v>44104.99998842592</v>
+        <v>44111.99998842592</v>
       </c>
       <c r="D9" t="n">
-        <v>1.17</v>
+        <v>1.5</v>
       </c>
       <c r="E9" t="n">
-        <v>1.03</v>
+        <v>1.09</v>
       </c>
       <c r="F9" t="n">
-        <v>1.5</v>
+        <v>1.75</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
-        <v>44091</v>
+        <v>44098</v>
       </c>
       <c r="B10" s="2" t="n">
-        <v>44104</v>
+        <v>44111</v>
       </c>
       <c r="C10" s="2" t="n">
-        <v>44097.99998842592</v>
+        <v>44104.99998842592</v>
       </c>
       <c r="D10" t="n">
-        <v>1.06</v>
+        <v>1.17</v>
       </c>
       <c r="E10" t="n">
-        <v>0.97</v>
+        <v>1.03</v>
       </c>
       <c r="F10" t="n">
-        <v>1.16</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
-        <v>44084</v>
+        <v>44091</v>
       </c>
       <c r="B11" s="2" t="n">
-        <v>44097</v>
+        <v>44104</v>
       </c>
       <c r="C11" s="2" t="n">
-        <v>44090.99998842592</v>
+        <v>44097.99998842592</v>
       </c>
       <c r="D11" t="n">
-        <v>1.01</v>
+        <v>1.06</v>
       </c>
       <c r="E11" t="n">
-        <v>0.88</v>
+        <v>0.97</v>
       </c>
       <c r="F11" t="n">
-        <v>1.08</v>
+        <v>1.16</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
-        <v>44077</v>
+        <v>44084</v>
       </c>
       <c r="B12" s="2" t="n">
-        <v>44090</v>
+        <v>44097</v>
       </c>
       <c r="C12" s="2" t="n">
-        <v>44083.99998842592</v>
+        <v>44090.99998842592</v>
       </c>
       <c r="D12" t="n">
-        <v>0.95</v>
+        <v>1.01</v>
       </c>
       <c r="E12" t="n">
         <v>0.88</v>
       </c>
       <c r="F12" t="n">
-        <v>1.05</v>
+        <v>1.08</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
-        <v>44070</v>
+        <v>44077</v>
       </c>
       <c r="B13" s="2" t="n">
-        <v>44083</v>
+        <v>44090</v>
       </c>
       <c r="C13" s="2" t="n">
-        <v>44076.99998842592</v>
+        <v>44083.99998842592</v>
       </c>
       <c r="D13" t="n">
-        <v>0.92</v>
+        <v>0.95</v>
       </c>
       <c r="E13" t="n">
-        <v>0.79</v>
+        <v>0.88</v>
       </c>
       <c r="F13" t="n">
-        <v>1.17</v>
+        <v>1.05</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
-        <v>44063</v>
+        <v>44070</v>
       </c>
       <c r="B14" s="2" t="n">
-        <v>44076</v>
+        <v>44083</v>
       </c>
       <c r="C14" s="2" t="n">
-        <v>44069.99998842592</v>
+        <v>44076.99998842592</v>
       </c>
       <c r="D14" t="n">
-        <v>1.14</v>
+        <v>0.92</v>
       </c>
       <c r="E14" t="n">
-        <v>0.71</v>
+        <v>0.79</v>
       </c>
       <c r="F14" t="n">
-        <v>1.53</v>
+        <v>1.17</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
-        <v>44056</v>
+        <v>44063</v>
       </c>
       <c r="B15" s="2" t="n">
-        <v>44069</v>
+        <v>44076</v>
       </c>
       <c r="C15" s="2" t="n">
-        <v>44062.99998842592</v>
+        <v>44069.99998842592</v>
       </c>
       <c r="D15" t="n">
-        <v>1.18</v>
+        <v>1.14</v>
       </c>
       <c r="E15" t="n">
-        <v>0.86</v>
+        <v>0.71</v>
       </c>
       <c r="F15" t="n">
-        <v>1.43</v>
+        <v>1.53</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
-        <v>44049</v>
+        <v>44056</v>
       </c>
       <c r="B16" s="2" t="n">
-        <v>44062</v>
+        <v>44069</v>
       </c>
       <c r="C16" s="2" t="n">
-        <v>44055.99998842592</v>
+        <v>44062.99998842592</v>
       </c>
       <c r="D16" t="n">
-        <v>0.75</v>
+        <v>1.18</v>
       </c>
       <c r="E16" t="n">
-        <v>0.52</v>
+        <v>0.86</v>
       </c>
       <c r="F16" t="n">
-        <v>1.24</v>
+        <v>1.43</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
-        <v>44042</v>
+        <v>44049</v>
       </c>
       <c r="B17" s="2" t="n">
-        <v>44055</v>
+        <v>44062</v>
       </c>
       <c r="C17" s="2" t="n">
-        <v>44048.99998842592</v>
+        <v>44055.99998842592</v>
       </c>
       <c r="D17" t="n">
-        <v>0.83</v>
+        <v>0.75</v>
       </c>
       <c r="E17" t="n">
-        <v>0.67</v>
+        <v>0.52</v>
       </c>
       <c r="F17" t="n">
-        <v>1.06</v>
+        <v>1.24</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
+        <v>44042</v>
+      </c>
+      <c r="B18" s="2" t="n">
+        <v>44055</v>
+      </c>
+      <c r="C18" s="2" t="n">
+        <v>44048.99998842592</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0.83</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0.67</v>
+      </c>
+      <c r="F18" t="n">
+        <v>1.06</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="2" t="n">
         <v>44035</v>
       </c>
-      <c r="B18" s="2" t="n">
+      <c r="B19" s="2" t="n">
         <v>44048</v>
       </c>
-      <c r="C18" s="2" t="n">
+      <c r="C19" s="2" t="n">
         <v>44041.99998842592</v>
       </c>
-      <c r="D18" t="n">
+      <c r="D19" t="n">
         <v>0.96</v>
       </c>
-      <c r="E18" t="n">
+      <c r="E19" t="n">
         <v>0.75</v>
       </c>
-      <c r="F18" t="n">
+      <c r="F19" t="n">
         <v>1.2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ISS update Dec 18
</commit_message>
<xml_diff>
--- a/data/computed/Rt_from_ISS_processed.xlsx
+++ b/data/computed/Rt_from_ISS_processed.xlsx
@@ -430,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -472,361 +472,381 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>44153</v>
+        <v>44160</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>44166</v>
+        <v>44173</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>44159.99998842592</v>
+        <v>44166.99930555555</v>
       </c>
       <c r="D2" t="n">
-        <v>0.82</v>
+        <v>0.86</v>
       </c>
       <c r="E2" t="n">
-        <v>0.76</v>
+        <v>0.79</v>
       </c>
       <c r="F2" t="n">
-        <v>0.91</v>
+        <v>0.9399999999999999</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>44146</v>
+        <v>44153</v>
       </c>
       <c r="B3" s="2" t="n">
-        <v>44159</v>
+        <v>44166</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>44152.99998842592</v>
+        <v>44159.99930555555</v>
       </c>
       <c r="D3" t="n">
+        <v>0.82</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.76</v>
+      </c>
+      <c r="F3" t="n">
         <v>0.91</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0.79</v>
-      </c>
-      <c r="F3" t="n">
-        <v>1.08</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>44139</v>
+        <v>44146</v>
       </c>
       <c r="B4" s="2" t="n">
-        <v>44152</v>
+        <v>44159</v>
       </c>
       <c r="C4" s="2" t="n">
-        <v>44145.99998842592</v>
+        <v>44152.99930555555</v>
       </c>
       <c r="D4" t="n">
+        <v>0.91</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.79</v>
+      </c>
+      <c r="F4" t="n">
         <v>1.08</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0.91</v>
-      </c>
-      <c r="F4" t="n">
-        <v>1.25</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>44132</v>
+        <v>44139</v>
       </c>
       <c r="B5" s="2" t="n">
-        <v>44145</v>
+        <v>44152</v>
       </c>
       <c r="C5" s="2" t="n">
-        <v>44138.99998842592</v>
+        <v>44145.99930555555</v>
       </c>
       <c r="D5" t="n">
-        <v>1.18</v>
+        <v>1.08</v>
       </c>
       <c r="E5" t="n">
-        <v>0.9399999999999999</v>
+        <v>0.91</v>
       </c>
       <c r="F5" t="n">
-        <v>1.49</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
-        <v>44126</v>
+        <v>44132</v>
       </c>
       <c r="B6" s="2" t="n">
-        <v>44139</v>
+        <v>44145</v>
       </c>
       <c r="C6" s="2" t="n">
-        <v>44132.99998842592</v>
+        <v>44138.99930555555</v>
       </c>
       <c r="D6" t="n">
-        <v>1.43</v>
+        <v>1.18</v>
       </c>
       <c r="E6" t="n">
-        <v>1.08</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="F6" t="n">
-        <v>1.81</v>
+        <v>1.49</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
-        <v>44119</v>
+        <v>44126</v>
       </c>
       <c r="B7" s="2" t="n">
-        <v>44132</v>
+        <v>44139</v>
       </c>
       <c r="C7" s="2" t="n">
-        <v>44125.99998842592</v>
+        <v>44132.99930555555</v>
       </c>
       <c r="D7" t="n">
-        <v>1.72</v>
+        <v>1.43</v>
       </c>
       <c r="E7" t="n">
-        <v>1.45</v>
+        <v>1.08</v>
       </c>
       <c r="F7" t="n">
-        <v>1.83</v>
+        <v>1.81</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
-        <v>44112</v>
+        <v>44119</v>
       </c>
       <c r="B8" s="2" t="n">
-        <v>44125</v>
+        <v>44132</v>
       </c>
       <c r="C8" s="2" t="n">
-        <v>44118.99998842592</v>
+        <v>44125.99930555555</v>
       </c>
       <c r="D8" t="n">
-        <v>1.7</v>
+        <v>1.72</v>
       </c>
       <c r="E8" t="n">
-        <v>1.49</v>
+        <v>1.45</v>
       </c>
       <c r="F8" t="n">
-        <v>1.85</v>
+        <v>1.83</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
-        <v>44105</v>
+        <v>44112</v>
       </c>
       <c r="B9" s="2" t="n">
-        <v>44118</v>
+        <v>44125</v>
       </c>
       <c r="C9" s="2" t="n">
-        <v>44111.99998842592</v>
+        <v>44118.99930555555</v>
       </c>
       <c r="D9" t="n">
-        <v>1.5</v>
+        <v>1.7</v>
       </c>
       <c r="E9" t="n">
-        <v>1.09</v>
+        <v>1.49</v>
       </c>
       <c r="F9" t="n">
-        <v>1.75</v>
+        <v>1.85</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
-        <v>44098</v>
+        <v>44105</v>
       </c>
       <c r="B10" s="2" t="n">
-        <v>44111</v>
+        <v>44118</v>
       </c>
       <c r="C10" s="2" t="n">
-        <v>44104.99998842592</v>
+        <v>44111.99930555555</v>
       </c>
       <c r="D10" t="n">
-        <v>1.17</v>
+        <v>1.5</v>
       </c>
       <c r="E10" t="n">
-        <v>1.03</v>
+        <v>1.09</v>
       </c>
       <c r="F10" t="n">
-        <v>1.5</v>
+        <v>1.75</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
-        <v>44091</v>
+        <v>44098</v>
       </c>
       <c r="B11" s="2" t="n">
-        <v>44104</v>
+        <v>44111</v>
       </c>
       <c r="C11" s="2" t="n">
-        <v>44097.99998842592</v>
+        <v>44104.99930555555</v>
       </c>
       <c r="D11" t="n">
-        <v>1.06</v>
+        <v>1.17</v>
       </c>
       <c r="E11" t="n">
-        <v>0.97</v>
+        <v>1.03</v>
       </c>
       <c r="F11" t="n">
-        <v>1.16</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
-        <v>44084</v>
+        <v>44091</v>
       </c>
       <c r="B12" s="2" t="n">
-        <v>44097</v>
+        <v>44104</v>
       </c>
       <c r="C12" s="2" t="n">
-        <v>44090.99998842592</v>
+        <v>44097.99930555555</v>
       </c>
       <c r="D12" t="n">
-        <v>1.01</v>
+        <v>1.06</v>
       </c>
       <c r="E12" t="n">
-        <v>0.88</v>
+        <v>0.97</v>
       </c>
       <c r="F12" t="n">
-        <v>1.08</v>
+        <v>1.16</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
-        <v>44077</v>
+        <v>44084</v>
       </c>
       <c r="B13" s="2" t="n">
-        <v>44090</v>
+        <v>44097</v>
       </c>
       <c r="C13" s="2" t="n">
-        <v>44083.99998842592</v>
+        <v>44090.99930555555</v>
       </c>
       <c r="D13" t="n">
-        <v>0.95</v>
+        <v>1.01</v>
       </c>
       <c r="E13" t="n">
         <v>0.88</v>
       </c>
       <c r="F13" t="n">
-        <v>1.05</v>
+        <v>1.08</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
-        <v>44070</v>
+        <v>44077</v>
       </c>
       <c r="B14" s="2" t="n">
-        <v>44083</v>
+        <v>44090</v>
       </c>
       <c r="C14" s="2" t="n">
-        <v>44076.99998842592</v>
+        <v>44083.99930555555</v>
       </c>
       <c r="D14" t="n">
-        <v>0.92</v>
+        <v>0.95</v>
       </c>
       <c r="E14" t="n">
-        <v>0.79</v>
+        <v>0.88</v>
       </c>
       <c r="F14" t="n">
-        <v>1.17</v>
+        <v>1.05</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
-        <v>44063</v>
+        <v>44070</v>
       </c>
       <c r="B15" s="2" t="n">
-        <v>44076</v>
+        <v>44083</v>
       </c>
       <c r="C15" s="2" t="n">
-        <v>44069.99998842592</v>
+        <v>44076.99930555555</v>
       </c>
       <c r="D15" t="n">
-        <v>1.14</v>
+        <v>0.92</v>
       </c>
       <c r="E15" t="n">
-        <v>0.71</v>
+        <v>0.79</v>
       </c>
       <c r="F15" t="n">
-        <v>1.53</v>
+        <v>1.17</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
-        <v>44056</v>
+        <v>44063</v>
       </c>
       <c r="B16" s="2" t="n">
-        <v>44069</v>
+        <v>44076</v>
       </c>
       <c r="C16" s="2" t="n">
-        <v>44062.99998842592</v>
+        <v>44069.99930555555</v>
       </c>
       <c r="D16" t="n">
-        <v>1.18</v>
+        <v>1.14</v>
       </c>
       <c r="E16" t="n">
-        <v>0.86</v>
+        <v>0.71</v>
       </c>
       <c r="F16" t="n">
-        <v>1.43</v>
+        <v>1.53</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
-        <v>44049</v>
+        <v>44056</v>
       </c>
       <c r="B17" s="2" t="n">
-        <v>44062</v>
+        <v>44069</v>
       </c>
       <c r="C17" s="2" t="n">
-        <v>44055.99998842592</v>
+        <v>44062.99930555555</v>
       </c>
       <c r="D17" t="n">
-        <v>0.75</v>
+        <v>1.18</v>
       </c>
       <c r="E17" t="n">
-        <v>0.52</v>
+        <v>0.86</v>
       </c>
       <c r="F17" t="n">
-        <v>1.24</v>
+        <v>1.43</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
-        <v>44042</v>
+        <v>44049</v>
       </c>
       <c r="B18" s="2" t="n">
-        <v>44055</v>
+        <v>44062</v>
       </c>
       <c r="C18" s="2" t="n">
-        <v>44048.99998842592</v>
+        <v>44055.99930555555</v>
       </c>
       <c r="D18" t="n">
-        <v>0.83</v>
+        <v>0.75</v>
       </c>
       <c r="E18" t="n">
-        <v>0.67</v>
+        <v>0.52</v>
       </c>
       <c r="F18" t="n">
-        <v>1.06</v>
+        <v>1.24</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="n">
+        <v>44042</v>
+      </c>
+      <c r="B19" s="2" t="n">
+        <v>44055</v>
+      </c>
+      <c r="C19" s="2" t="n">
+        <v>44048.99930555555</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0.83</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0.67</v>
+      </c>
+      <c r="F19" t="n">
+        <v>1.06</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="2" t="n">
         <v>44035</v>
       </c>
-      <c r="B19" s="2" t="n">
+      <c r="B20" s="2" t="n">
         <v>44048</v>
       </c>
-      <c r="C19" s="2" t="n">
-        <v>44041.99998842592</v>
-      </c>
-      <c r="D19" t="n">
+      <c r="C20" s="2" t="n">
+        <v>44041.99930555555</v>
+      </c>
+      <c r="D20" t="n">
         <v>0.96</v>
       </c>
-      <c r="E19" t="n">
+      <c r="E20" t="n">
         <v>0.75</v>
       </c>
-      <c r="F19" t="n">
+      <c r="F20" t="n">
         <v>1.2</v>
       </c>
     </row>

</xml_diff>